<commit_message>
Add main Image ver.
</commit_message>
<xml_diff>
--- a/data/result/result_all.xlsx
+++ b/data/result/result_all.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Desktop/映画評価データ/MovieRecommend/data/result/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1420" windowWidth="25520" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="4040" yWindow="1740" windowWidth="25520" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>Itembase</t>
     <phoneticPr fontId="1"/>
@@ -109,8 +104,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -128,13 +127,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -142,6 +143,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -475,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,11 +497,11 @@
         <v>32.46</v>
       </c>
       <c r="E1" s="1">
-        <f>ABS(C1-$C$7)</f>
+        <f>ABS(C1-$C$9)</f>
         <v>4.9400000000000013</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -509,11 +512,11 @@
         <v>62.67</v>
       </c>
       <c r="E2" s="1">
-        <f>ABS(C2-$C$8)</f>
+        <f>ABS(C2-$C$10)</f>
         <v>5.730000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -524,11 +527,11 @@
         <v>35.020000000000003</v>
       </c>
       <c r="E3" s="1">
-        <f>ABS(C3-$C$7)</f>
+        <f t="shared" ref="E3:E6" si="0">ABS(C3-$C$9)</f>
         <v>7.5000000000000036</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -539,11 +542,11 @@
         <v>65.81</v>
       </c>
       <c r="E4" s="1">
-        <f>ABS(C4-$C$8)</f>
+        <f t="shared" ref="E4:E6" si="1">ABS(C4-$C$10)</f>
         <v>8.8700000000000045</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -554,11 +557,11 @@
         <v>34.57</v>
       </c>
       <c r="E5" s="1">
-        <f>ABS(C5-$C$7)</f>
+        <f t="shared" ref="E5:E7" si="2">ABS(C5-$C$9)</f>
         <v>7.0500000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -569,29 +572,59 @@
         <v>64.02</v>
       </c>
       <c r="E6" s="1">
-        <f>ABS(C6-$C$8)</f>
+        <f t="shared" ref="E6:E8" si="3">ABS(C6-$C$10)</f>
         <v>7.0799999999999983</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>27.52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C7" s="1">
+        <v>33.66136765076962</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>6.1413676507696202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
+        <v>63.512490537471614</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="3"/>
+        <v>6.5724905374716158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>27.52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
         <v>56.94</v>
       </c>
     </row>
@@ -599,5 +632,10 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>